<commit_message>
New changes ot the project
</commit_message>
<xml_diff>
--- a/test-data/Testdata.xlsx
+++ b/test-data/Testdata.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/my_appie_pie/Documents/Selenium/workspaceNew/AvaamoProject/test-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/my_appie_pie/Documents/Selenium/workspaceNew/IRAAIProject/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28A2E37-8732-6A47-93FE-C1D716BB6123}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCB3DE1-EFA2-5D43-BFE5-F316CB33F15A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="680" windowWidth="27640" windowHeight="15740" activeTab="1" xr2:uid="{306626C2-B62F-0B41-BC84-4FF8D261F1F2}"/>
+    <workbookView xWindow="1160" yWindow="480" windowWidth="27640" windowHeight="15740" activeTab="2" xr2:uid="{306626C2-B62F-0B41-BC84-4FF8D261F1F2}"/>
   </bookViews>
   <sheets>
     <sheet name="fillform" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="renew_policy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>DATASET</t>
   </si>
@@ -122,16 +123,84 @@
   </si>
   <si>
     <t>Take care!</t>
+  </si>
+  <si>
+    <t>HR21AB1010</t>
+  </si>
+  <si>
+    <t>policyNo</t>
+  </si>
+  <si>
+    <t>registrationNo</t>
+  </si>
+  <si>
+    <t>MobileNo</t>
+  </si>
+  <si>
+    <t>emaild</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>renew policy1</t>
+  </si>
+  <si>
+    <t>M0012345</t>
+  </si>
+  <si>
+    <t>Policy Number</t>
+  </si>
+  <si>
+    <t>Vehicle Registration Number</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>renew header labels</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Option</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,10 +241,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -193,8 +263,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,7 +589,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,10 +646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F391875-D59B-5E46-95F3-3FEF3572030B}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,7 +737,95 @@
         <v>19</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A6DA0A-1DFF-294C-B7D9-D9F82098FAB6}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4">
+        <v>9857689500</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{39AAE4DB-4C33-9940-90BE-5F6BF24D2CC2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>